<commit_message>
Remove os índices da planilha a ser exportada
</commit_message>
<xml_diff>
--- a/BaseProdutosAtualizada.xlsx
+++ b/BaseProdutosAtualizada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,250 +434,229 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Produtos</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Produtos</t>
+          <t>Preço Original</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Preço Original</t>
+          <t>Moeda</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Moeda</t>
+          <t>Cotação</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Cotação</t>
+          <t>Preço de Compra</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Preço de Compra</t>
+          <t>Margem</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Margem</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
           <t>Preço de Venda</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>Câmera Canon</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="B2" t="n">
         <v>999.99</v>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Dólar</t>
         </is>
       </c>
+      <c r="D2" t="n">
+        <v>5.233274</v>
+      </c>
       <c r="E2" t="n">
-        <v>5.2332</v>
+        <v>5233.22166726</v>
       </c>
       <c r="F2" t="n">
-        <v>5233.147668000001</v>
+        <v>1.4</v>
       </c>
       <c r="G2" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="H2" t="n">
-        <v>7326.4067352</v>
+        <v>7326.510334163999</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>Carro Renault</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="B3" t="n">
         <v>4500</v>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Euro</t>
         </is>
       </c>
+      <c r="D3" t="n">
+        <v>5.5827</v>
+      </c>
       <c r="E3" t="n">
-        <v>5.57885286</v>
+        <v>25122.15</v>
       </c>
       <c r="F3" t="n">
-        <v>25104.83787</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
+        <v>50244.3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Notebook Dell</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>899.99</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Dólar</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5.233274</v>
+      </c>
+      <c r="E4" t="n">
+        <v>4709.89426726</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8006.820254341999</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>IPhone</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>799</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Dólar</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>5.233274</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4181.385926</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7108.3560742</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Carro Fiat</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>3000</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Euro</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>5.5827</v>
+      </c>
+      <c r="E6" t="n">
+        <v>16748.1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="G6" t="n">
+        <v>31821.39</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Celular Xiaomi</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>480.48</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Dólar</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>5.233274</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2514.48349152</v>
+      </c>
+      <c r="F7" t="n">
         <v>2</v>
       </c>
-      <c r="H3" t="n">
-        <v>50209.67574000001</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Notebook Dell</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>899.99</v>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Dólar</t>
-        </is>
-      </c>
-      <c r="E4" t="n">
-        <v>5.2332</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4709.827668</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="H4" t="n">
-        <v>8006.707035599999</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>IPhone</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>799</v>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Dólar</t>
-        </is>
-      </c>
-      <c r="E5" t="n">
-        <v>5.2332</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4181.3268</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1.7</v>
-      </c>
-      <c r="H5" t="n">
-        <v>7108.25556</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Carro Fiat</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Euro</t>
-        </is>
-      </c>
-      <c r="E6" t="n">
-        <v>5.57885286</v>
-      </c>
-      <c r="F6" t="n">
-        <v>16736.55858</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="H6" t="n">
-        <v>31799.461302</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Celular Xiaomi</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>480.48</v>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Dólar</t>
-        </is>
-      </c>
-      <c r="E7" t="n">
-        <v>5.2332</v>
-      </c>
-      <c r="F7" t="n">
-        <v>2514.447936</v>
-      </c>
       <c r="G7" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" t="n">
-        <v>5028.895872</v>
+        <v>5028.96698304</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>Joia 20g</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="B8" t="n">
         <v>20</v>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Ouro</t>
         </is>
       </c>
+      <c r="D8" t="n">
+        <v>310.42</v>
+      </c>
       <c r="E8" t="n">
-        <v>309.97</v>
+        <v>6208.400000000001</v>
       </c>
       <c r="F8" t="n">
-        <v>6199.400000000001</v>
+        <v>1.15</v>
       </c>
       <c r="G8" t="n">
-        <v>1.15</v>
-      </c>
-      <c r="H8" t="n">
-        <v>7129.31</v>
+        <v>7139.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>